<commit_message>
upload new excel file with test data
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/TestData.xlsx
+++ b/src/test/java/testdata/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C571BC5-44AD-4DFB-A9DC-4B5F77FA8A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612CE102-E858-478B-B176-EE127386FBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="690" windowWidth="20490" windowHeight="10770" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
     <sheet name="CATSLogin" sheetId="12" r:id="rId2"/>
+    <sheet name="AgentLogin" sheetId="13" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>don1thack</t>
   </si>
@@ -65,9 +66,6 @@
     <t>CustomerNum</t>
   </si>
   <si>
-    <t>53357214</t>
-  </si>
-  <si>
     <t>SendLettersbyMail</t>
   </si>
   <si>
@@ -89,18 +87,12 @@
     <t>No</t>
   </si>
   <si>
-    <t>011000015</t>
-  </si>
-  <si>
     <t>BankAccountNum</t>
   </si>
   <si>
     <t>ReenterBankAccountNum</t>
   </si>
   <si>
-    <t>12345</t>
-  </si>
-  <si>
     <t>BankAccountType</t>
   </si>
   <si>
@@ -116,7 +108,13 @@
     <t>CalendarDay</t>
   </si>
   <si>
-    <t>13</t>
+    <t>HEALTHBENEFI</t>
+  </si>
+  <si>
+    <t>LetterName</t>
+  </si>
+  <si>
+    <t>Ptest</t>
   </si>
 </sst>
 </file>
@@ -181,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -190,6 +188,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -537,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D071FE2-89C5-4C36-B925-609C062F8AEB}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,34 +569,34 @@
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -605,38 +606,38 @@
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
+      <c r="C2" s="6">
+        <v>53357214</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="H2" s="6">
+        <v>11000015</v>
+      </c>
+      <c r="I2" s="6">
+        <v>12345</v>
+      </c>
+      <c r="J2" s="6">
+        <v>12345</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="M2" s="6">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -644,4 +645,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A6EE5C-BA51-4480-B29C-8CA8A4F57F00}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Census screen TC commit
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/TestData.xlsx
+++ b/src/test/java/testdata/TestData.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9935B6-17CF-421E-8A15-3CFCC4D6660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2EF721-028F-4308-AD15-1285CE919A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
     <sheet name="CATSLogin" sheetId="12" r:id="rId2"/>
     <sheet name="Census" sheetId="14" r:id="rId3"/>
     <sheet name="AgentLogin" sheetId="13" r:id="rId4"/>
+    <sheet name="EmpQuotes" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>don1thack</t>
   </si>
@@ -296,6 +297,12 @@
   </si>
   <si>
     <t>28</t>
+  </si>
+  <si>
+    <t>QuoteNbr</t>
+  </si>
+  <si>
+    <t>23,24</t>
   </si>
 </sst>
 </file>
@@ -360,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -374,6 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E889C558-029C-4152-BA50-B7DC4E459171}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,4 +1088,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77307AAB-B7AD-4648-A342-07AC570533BE}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Push new branch including Group Details test , Emp group Quotes test and Group Roaster test
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/TestData.xlsx
+++ b/src/test/java/testdata/TestData.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2EF721-028F-4308-AD15-1285CE919A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DEBC7C-2310-49B2-A16B-93D991A40E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
-    <sheet name="CATSLogin" sheetId="12" r:id="rId2"/>
-    <sheet name="Census" sheetId="14" r:id="rId3"/>
-    <sheet name="AgentLogin" sheetId="13" r:id="rId4"/>
-    <sheet name="EmpQuotes" sheetId="15" r:id="rId5"/>
+    <sheet name="GroupRoaster" sheetId="16" r:id="rId2"/>
+    <sheet name="CATSLogin" sheetId="12" r:id="rId3"/>
+    <sheet name="Census" sheetId="14" r:id="rId4"/>
+    <sheet name="AgentLogin" sheetId="13" r:id="rId5"/>
+    <sheet name="EmpQuotes" sheetId="15" r:id="rId6"/>
+    <sheet name="GroupDetails" sheetId="18" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="127">
   <si>
     <t>don1thack</t>
   </si>
@@ -302,14 +304,116 @@
     <t>QuoteNbr</t>
   </si>
   <si>
-    <t>23,24</t>
+    <t>CompleteOnline</t>
+  </si>
+  <si>
+    <t>SubmitCompleteApplications</t>
+  </si>
+  <si>
+    <t>Agent_Chk</t>
+  </si>
+  <si>
+    <t>Emp_Grp</t>
+  </si>
+  <si>
+    <t>Grp_Email</t>
+  </si>
+  <si>
+    <t>denFlag</t>
+  </si>
+  <si>
+    <t>blFlag</t>
+  </si>
+  <si>
+    <t>stdFlag</t>
+  </si>
+  <si>
+    <t>visFlag</t>
+  </si>
+  <si>
+    <t>vlFlag</t>
+  </si>
+  <si>
+    <t>dvFlag</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>empPath</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>D:\Local\Git\CatsAuto\Autoit\RoasterFileUpload.exe</t>
+  </si>
+  <si>
+    <t>D:\Local\Git\CatsAuto\Autoit\EmpRoasterFileUpload.exe</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>CustName</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>SICcode</t>
+  </si>
+  <si>
+    <t>PayrollNum</t>
+  </si>
+  <si>
+    <t>test2023</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>test address 2</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>SelectChk</t>
+  </si>
+  <si>
+    <t>6035</t>
+  </si>
+  <si>
+    <t>35202</t>
+  </si>
+  <si>
+    <t>Dental,Life - Basic,LTD,Vision</t>
+  </si>
+  <si>
+    <t>53570004</t>
+  </si>
+  <si>
+    <t>19,20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +431,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,26 +476,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,7 +810,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -724,11 +837,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190FFED8-CAA3-4624-97C4-E12EEFF7AA6D}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" activeCellId="1" sqref="A2 B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{2F188504-FB06-4279-93CD-9FA51BE475AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D071FE2-89C5-4C36-B925-609C062F8AEB}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,43 +1028,43 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="4">
         <v>12345</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="4">
         <v>12345</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="4">
         <v>13</v>
       </c>
     </row>
@@ -836,7 +1075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E889C558-029C-4152-BA50-B7DC4E459171}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
@@ -947,97 +1186,97 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AB2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AC2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AD2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AE2" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1047,7 +1286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A6EE5C-BA51-4480-B29C-8CA8A4F57F00}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1074,13 +1313,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1090,15 +1329,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77307AAB-B7AD-4648-A342-07AC570533BE}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -1115,17 +1357,100 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>92</v>
+      <c r="C2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E776B54E-5FBF-445D-B4A9-C993708E7758}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>